<commit_message>
Greatest update since ever
</commit_message>
<xml_diff>
--- a/docs/level-formula.xlsx
+++ b/docs/level-formula.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\empoweredpixels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\empoweredpixels\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D484FB11-424E-4536-94AE-08313FABC2FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0E8934-DD28-4BF5-812B-BDB082EAF93C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{92CA5BE5-4720-48AC-92F2-B4DBCF2AD469}"/>
+    <workbookView xWindow="5388" yWindow="1020" windowWidth="17280" windowHeight="8964" xr2:uid="{92CA5BE5-4720-48AC-92F2-B4DBCF2AD469}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Lv</t>
   </si>
@@ -56,13 +56,16 @@
   <si>
     <t>Days</t>
   </si>
+  <si>
+    <t>Cumulated</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -95,7 +98,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -411,18 +414,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5ABDCA2-575D-45C7-B8E9-44ED6DAFE5F6}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,59 +433,70 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f>$E$2*(($E$4* A2/8)^2)</f>
+        <f>$F$2*(($F$4* A2/8)^2)</f>
         <v>500</v>
       </c>
       <c r="C2" s="2">
-        <f>B2/$E$3</f>
+        <f>SUM(B$2:B2)</f>
+        <v>500</v>
+      </c>
+      <c r="D2" s="2">
+        <f>B2/$F$3</f>
         <v>1.25</v>
       </c>
-      <c r="D2" s="1">
-        <f>C2/$E$5</f>
+      <c r="E2" s="1">
+        <f>D2/$F$5</f>
         <v>0.15625</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>5120</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B33" si="0">$E$2*(($E$4* A3/8)^2)</f>
+        <f t="shared" ref="B3:B33" si="0">$F$2*(($F$4* A3/8)^2)</f>
         <v>2000</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C33" si="1">B3/$E$3</f>
+        <f>SUM(B$2:B3)</f>
+        <v>2500</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D33" si="1">B3/$F$3</f>
         <v>5</v>
       </c>
-      <c r="D3" s="1">
-        <f>(C3/$E$5)+D2</f>
+      <c r="E3" s="1">
+        <f>(D3/$F$5)+E2</f>
         <v>0.78125</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>400</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -491,21 +505,25 @@
         <v>4500</v>
       </c>
       <c r="C4" s="2">
+        <f>SUM(B$2:B4)</f>
+        <v>7000</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="1"/>
         <v>11.25</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" ref="D4:D33" si="2">(C4/$E$5)+D3</f>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4:E33" si="2">(D4/$F$5)+E3</f>
         <v>2.1875</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2.5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -514,21 +532,25 @@
         <v>8000</v>
       </c>
       <c r="C5" s="2">
+        <f>SUM(B$2:B5)</f>
+        <v>15000</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <f t="shared" si="2"/>
         <v>4.6875</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>8</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -537,15 +559,19 @@
         <v>12500</v>
       </c>
       <c r="C6" s="2">
+        <f>SUM(B$2:B6)</f>
+        <v>27500</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" si="1"/>
         <v>31.25</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <f t="shared" si="2"/>
         <v>8.59375</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -554,15 +580,19 @@
         <v>18000</v>
       </c>
       <c r="C7" s="2">
+        <f>SUM(B$2:B7)</f>
+        <v>45500</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <f t="shared" si="2"/>
         <v>14.21875</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -571,15 +601,19 @@
         <v>24500</v>
       </c>
       <c r="C8" s="2">
+        <f>SUM(B$2:B8)</f>
+        <v>70000</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="1"/>
         <v>61.25</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <f t="shared" si="2"/>
         <v>21.875</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -588,15 +622,19 @@
         <v>32000</v>
       </c>
       <c r="C9" s="2">
+        <f>SUM(B$2:B9)</f>
+        <v>102000</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <f t="shared" si="2"/>
         <v>31.875</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -605,15 +643,19 @@
         <v>40500</v>
       </c>
       <c r="C10" s="2">
+        <f>SUM(B$2:B10)</f>
+        <v>142500</v>
+      </c>
+      <c r="D10" s="2">
         <f t="shared" si="1"/>
         <v>101.25</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <f t="shared" si="2"/>
         <v>44.53125</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -622,15 +664,19 @@
         <v>50000</v>
       </c>
       <c r="C11" s="2">
+        <f>SUM(B$2:B11)</f>
+        <v>192500</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
         <v>60.15625</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -639,15 +685,19 @@
         <v>60500</v>
       </c>
       <c r="C12" s="2">
+        <f>SUM(B$2:B12)</f>
+        <v>253000</v>
+      </c>
+      <c r="D12" s="2">
         <f t="shared" si="1"/>
         <v>151.25</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <f t="shared" si="2"/>
         <v>79.0625</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -656,15 +706,19 @@
         <v>72000</v>
       </c>
       <c r="C13" s="2">
+        <f>SUM(B$2:B13)</f>
+        <v>325000</v>
+      </c>
+      <c r="D13" s="2">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <f t="shared" si="2"/>
         <v>101.5625</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -673,15 +727,19 @@
         <v>84500</v>
       </c>
       <c r="C14" s="2">
+        <f>SUM(B$2:B14)</f>
+        <v>409500</v>
+      </c>
+      <c r="D14" s="2">
         <f t="shared" si="1"/>
         <v>211.25</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <f t="shared" si="2"/>
         <v>127.96875</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -690,15 +748,19 @@
         <v>98000</v>
       </c>
       <c r="C15" s="2">
+        <f>SUM(B$2:B15)</f>
+        <v>507500</v>
+      </c>
+      <c r="D15" s="2">
         <f t="shared" si="1"/>
         <v>245</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <f t="shared" si="2"/>
         <v>158.59375</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -707,15 +769,19 @@
         <v>112500</v>
       </c>
       <c r="C16" s="2">
+        <f>SUM(B$2:B16)</f>
+        <v>620000</v>
+      </c>
+      <c r="D16" s="2">
         <f t="shared" si="1"/>
         <v>281.25</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <f t="shared" si="2"/>
         <v>193.75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -724,15 +790,19 @@
         <v>128000</v>
       </c>
       <c r="C17" s="2">
+        <f>SUM(B$2:B17)</f>
+        <v>748000</v>
+      </c>
+      <c r="D17" s="2">
         <f t="shared" si="1"/>
         <v>320</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <f t="shared" si="2"/>
         <v>233.75</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -741,15 +811,19 @@
         <v>144500</v>
       </c>
       <c r="C18" s="2">
+        <f>SUM(B$2:B18)</f>
+        <v>892500</v>
+      </c>
+      <c r="D18" s="2">
         <f t="shared" si="1"/>
         <v>361.25</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <f t="shared" si="2"/>
         <v>278.90625</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -758,15 +832,19 @@
         <v>162000</v>
       </c>
       <c r="C19" s="2">
+        <f>SUM(B$2:B19)</f>
+        <v>1054500</v>
+      </c>
+      <c r="D19" s="2">
         <f t="shared" si="1"/>
         <v>405</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <f t="shared" si="2"/>
         <v>329.53125</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -775,15 +853,19 @@
         <v>180500</v>
       </c>
       <c r="C20" s="2">
+        <f>SUM(B$2:B20)</f>
+        <v>1235000</v>
+      </c>
+      <c r="D20" s="2">
         <f t="shared" si="1"/>
         <v>451.25</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <f t="shared" si="2"/>
         <v>385.9375</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -792,15 +874,19 @@
         <v>200000</v>
       </c>
       <c r="C21" s="2">
+        <f>SUM(B$2:B21)</f>
+        <v>1435000</v>
+      </c>
+      <c r="D21" s="2">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <f t="shared" si="2"/>
         <v>448.4375</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -809,15 +895,19 @@
         <v>220500</v>
       </c>
       <c r="C22" s="2">
+        <f>SUM(B$2:B22)</f>
+        <v>1655500</v>
+      </c>
+      <c r="D22" s="2">
         <f t="shared" si="1"/>
         <v>551.25</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <f t="shared" si="2"/>
         <v>517.34375</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -826,15 +916,19 @@
         <v>242000</v>
       </c>
       <c r="C23" s="2">
+        <f>SUM(B$2:B23)</f>
+        <v>1897500</v>
+      </c>
+      <c r="D23" s="2">
         <f t="shared" si="1"/>
         <v>605</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <f t="shared" si="2"/>
         <v>592.96875</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -843,15 +937,19 @@
         <v>264500</v>
       </c>
       <c r="C24" s="2">
+        <f>SUM(B$2:B24)</f>
+        <v>2162000</v>
+      </c>
+      <c r="D24" s="2">
         <f t="shared" si="1"/>
         <v>661.25</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <f t="shared" si="2"/>
         <v>675.625</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -860,15 +958,19 @@
         <v>288000</v>
       </c>
       <c r="C25" s="2">
+        <f>SUM(B$2:B25)</f>
+        <v>2450000</v>
+      </c>
+      <c r="D25" s="2">
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <f t="shared" si="2"/>
         <v>765.625</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -877,15 +979,19 @@
         <v>312500</v>
       </c>
       <c r="C26" s="2">
+        <f>SUM(B$2:B26)</f>
+        <v>2762500</v>
+      </c>
+      <c r="D26" s="2">
         <f t="shared" si="1"/>
         <v>781.25</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <f t="shared" si="2"/>
         <v>863.28125</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -894,15 +1000,19 @@
         <v>338000</v>
       </c>
       <c r="C27" s="2">
+        <f>SUM(B$2:B27)</f>
+        <v>3100500</v>
+      </c>
+      <c r="D27" s="2">
         <f t="shared" si="1"/>
         <v>845</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <f t="shared" si="2"/>
         <v>968.90625</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -911,15 +1021,19 @@
         <v>364500</v>
       </c>
       <c r="C28" s="2">
+        <f>SUM(B$2:B28)</f>
+        <v>3465000</v>
+      </c>
+      <c r="D28" s="2">
         <f t="shared" si="1"/>
         <v>911.25</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <f t="shared" si="2"/>
         <v>1082.8125</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -928,15 +1042,19 @@
         <v>392000</v>
       </c>
       <c r="C29" s="2">
+        <f>SUM(B$2:B29)</f>
+        <v>3857000</v>
+      </c>
+      <c r="D29" s="2">
         <f t="shared" si="1"/>
         <v>980</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <f t="shared" si="2"/>
         <v>1205.3125</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -945,15 +1063,19 @@
         <v>420500</v>
       </c>
       <c r="C30" s="2">
+        <f>SUM(B$2:B30)</f>
+        <v>4277500</v>
+      </c>
+      <c r="D30" s="2">
         <f t="shared" si="1"/>
         <v>1051.25</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <f t="shared" si="2"/>
         <v>1336.71875</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -962,15 +1084,19 @@
         <v>450000</v>
       </c>
       <c r="C31" s="2">
+        <f>SUM(B$2:B31)</f>
+        <v>4727500</v>
+      </c>
+      <c r="D31" s="2">
         <f t="shared" si="1"/>
         <v>1125</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <f t="shared" si="2"/>
         <v>1477.34375</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -979,15 +1105,19 @@
         <v>480500</v>
       </c>
       <c r="C32" s="2">
+        <f>SUM(B$2:B32)</f>
+        <v>5208000</v>
+      </c>
+      <c r="D32" s="2">
         <f t="shared" si="1"/>
         <v>1201.25</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <f t="shared" si="2"/>
         <v>1627.5</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -996,21 +1126,26 @@
         <v>512000</v>
       </c>
       <c r="C33" s="2">
+        <f>SUM(B$2:B33)</f>
+        <v>5720000</v>
+      </c>
+      <c r="D33" s="2">
         <f t="shared" si="1"/>
         <v>1280</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <f t="shared" si="2"/>
         <v>1787.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <f>SUM(B2:B33)</f>
         <v>5720000</v>
       </c>
-      <c r="C35" s="2">
-        <f>SUM(C2:C33)</f>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2">
+        <f>SUM(D2:D33)</f>
         <v>14300</v>
       </c>
     </row>

</xml_diff>